<commit_message>
10/29 changes and updates
</commit_message>
<xml_diff>
--- a/Square Mileage.xlsx
+++ b/Square Mileage.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26500" windowHeight="16620" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -267,10 +267,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -575,6 +581,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1424,6 +1433,8 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="61" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>